<commit_message>
Gjorde ändringar till UML filem och index
</commit_message>
<xml_diff>
--- a/Structure/UML.xlsx
+++ b/Structure/UML.xlsx
@@ -510,7 +510,7 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,7 +789,7 @@
         <v>42</v>
       </c>
       <c r="C42" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -800,7 +800,7 @@
         <v>44</v>
       </c>
       <c r="C43" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>